<commit_message>
Replacing old data files with formatted files
</commit_message>
<xml_diff>
--- a/b04.xlsx
+++ b/b04.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kasarayv\Downloads\iot\reports\final\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0C394B-C486-4099-9E05-39DF805FED58}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="20370" yWindow="-3960" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="area" sheetId="1" r:id="rId1"/>
     <sheet name="power" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
     <t>RN</t>
   </si>
@@ -27,14 +33,37 @@
   </si>
   <si>
     <t>DS</t>
+  </si>
+  <si>
+    <t>Technique</t>
+  </si>
+  <si>
+    <t>KeySize=32</t>
+  </si>
+  <si>
+    <t>KeySize=64</t>
+  </si>
+  <si>
+    <t>KeySize=128</t>
+  </si>
+  <si>
+    <t>KeySize=256</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -62,14 +91,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -116,7 +159,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -148,9 +191,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -182,6 +243,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -357,91 +436,98 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:E5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0.01</v>
-      </c>
-      <c r="C2">
-        <v>-0.005823846527109229</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>-0.01303181474407248</v>
-      </c>
-      <c r="F2">
-        <v>-0.003838380557669951</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>-5.8238465271092292E-3</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>-1.303181474407248E-2</v>
+      </c>
+      <c r="E2" s="2">
+        <v>-3.8383805576699512E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>0.01</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>-0.001519441339167734</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>-1.5194413391677339E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>0.01</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>-0.00484706254849724</v>
-      </c>
-      <c r="F4">
-        <v>-0.004988126673334875</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>-4.8470625484972399E-3</v>
+      </c>
+      <c r="E4" s="2">
+        <v>-4.9881266733348747E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>0.01</v>
-      </c>
-      <c r="C5">
-        <v>0.08793274191652793</v>
-      </c>
-      <c r="D5">
-        <v>0.08793274191652793</v>
-      </c>
-      <c r="E5">
-        <v>0.08637708853374489</v>
-      </c>
-      <c r="F5">
-        <v>0.08187471214896049</v>
+      <c r="B5" s="2">
+        <v>8.7932741916527932E-2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>8.7932741916527932E-2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>8.6377088533744886E-2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>8.1874712148960485E-2</v>
       </c>
     </row>
   </sheetData>
@@ -450,91 +536,98 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:E5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0.01</v>
-      </c>
-      <c r="C2">
-        <v>0.001088423612898469</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0.003543074266247297</v>
-      </c>
-      <c r="F2">
-        <v>0.02383333366077732</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1.088423612898469E-3</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>3.543074266247297E-3</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2.383333366077732E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>0.01</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0.02131267031177249</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2.1312670311772489E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>0.01</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>-0.002941887216523548</v>
-      </c>
-      <c r="F4">
-        <v>0.01501395893460224</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>-2.941887216523548E-3</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1.501395893460224E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>0.01</v>
-      </c>
-      <c r="C5">
-        <v>0.05842398618448591</v>
-      </c>
-      <c r="D5">
-        <v>0.05887664466898357</v>
-      </c>
-      <c r="E5">
-        <v>0.04237622128398616</v>
-      </c>
-      <c r="F5">
-        <v>0.02285178774560758</v>
+      <c r="B5" s="2">
+        <v>5.842398618448591E-2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>5.8876644668983569E-2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>4.237622128398616E-2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2.2851787745607581E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>